<commit_message>
let xlsx to be online env, also modify npm test command
</commit_message>
<xml_diff>
--- a/issuedGUI.xlsx
+++ b/issuedGUI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="文字" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,11 @@
     <sheet name="文字映射" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="80">
   <si>
     <t>http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html</t>
   </si>
@@ -347,9 +346,6 @@
     <t>.s-masonry dl dt a</t>
   </si>
   <si>
-    <t>http://test.item.www.milanoo.com/</t>
-  </si>
-  <si>
     <t>.s-masonry dl dd a</t>
   </si>
   <si>
@@ -399,6 +395,12 @@
   </si>
   <si>
     <t>Word20</t>
+  </si>
+  <si>
+    <t>http://www.milanoo.com/product/full-skirt-vintage-dress-p538381.html</t>
+  </si>
+  <si>
+    <t>http://www.milanoo.com/</t>
   </si>
 </sst>
 </file>
@@ -792,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,7 +818,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -825,7 +827,7 @@
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -836,7 +838,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -847,21 +849,21 @@
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
         <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -869,10 +871,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -880,10 +882,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -891,10 +893,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -902,10 +904,10 @@
         <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -913,10 +915,10 @@
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -924,10 +926,10 @@
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -935,10 +937,10 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -946,10 +948,10 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -957,10 +959,10 @@
         <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -968,10 +970,10 @@
         <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -979,10 +981,10 @@
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -990,10 +992,10 @@
         <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1001,10 +1003,10 @@
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1012,10 +1014,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1023,31 +1025,31 @@
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://test.item.www.milanoo.com/"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://test.item.www.milanoo.com/"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://test.item.www.milanoo.com/"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://test.item.www.milanoo.com/"/>
+    <hyperlink ref="B7" r:id="rId6" display="http://test.item.www.milanoo.com/"/>
+    <hyperlink ref="B8" r:id="rId7" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B9" r:id="rId8" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B10" r:id="rId9" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B13" r:id="rId12" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B14" r:id="rId13" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
+    <hyperlink ref="B15" r:id="rId14" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
     <hyperlink ref="B16:B19" r:id="rId15" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
-    <hyperlink ref="B20" r:id="rId16"/>
+    <hyperlink ref="B20" r:id="rId16" display="http://test.item.www.milanoo.com/product/full-skirt-vintage-dress-p538381.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
@@ -1288,7 +1290,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,7 +1418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1464,7 +1466,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1696,7 +1698,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>

</xml_diff>